<commit_message>
Create all necessary folders and add example spreadsheet
</commit_message>
<xml_diff>
--- a/examples/Hong_3979_170316B1.xlsx
+++ b/examples/Hong_3979_170316B1.xlsx
@@ -357,9 +357,6 @@
     <t>Hong_3979_170316B1</t>
   </si>
   <si>
-    <t>0pfj7wGzbgUD</t>
-  </si>
-  <si>
     <t>1_Experimental</t>
   </si>
   <si>
@@ -637,6 +634,9 @@
   </si>
   <si>
     <t>broad</t>
+  </si>
+  <si>
+    <t>XXXXXX</t>
   </si>
 </sst>
 </file>
@@ -1000,87 +1000,7 @@
     <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1475,8 +1395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D49" workbookViewId="0">
-      <selection activeCell="K63" sqref="K63:K65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1524,13 +1444,13 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L1" t="s">
         <v>10</v>
@@ -1544,26 +1464,26 @@
         <v>109</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D2" t="str">
         <f>CONCATENATE("Sample_",E2,"")</f>
         <v>Sample_1_Experimental</v>
       </c>
       <c r="E2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -1577,26 +1497,26 @@
         <v>109</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D3" t="str">
         <f>CONCATENATE("Sample_",E3,"")</f>
         <v>Sample_2_Experimental</v>
       </c>
       <c r="E3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -1609,26 +1529,26 @@
         <v>109</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" ref="D4:D67" si="0">CONCATENATE("Sample_",E4,"")</f>
         <v>Sample_3_Experimental</v>
       </c>
       <c r="E4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
@@ -1645,26 +1565,26 @@
         <v>109</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-3 0hr</v>
       </c>
       <c r="E5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
       </c>
       <c r="G5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K5" s="4"/>
       <c r="Q5" s="1"/>
@@ -1678,26 +1598,26 @@
         <v>109</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-3 1hr</v>
       </c>
       <c r="E6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K6" s="4"/>
       <c r="Q6" s="1"/>
@@ -1711,26 +1631,26 @@
         <v>109</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
         <v>Sample_6_Control</v>
       </c>
       <c r="E7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K7" s="4"/>
       <c r="Q7" s="1"/>
@@ -1744,26 +1664,26 @@
         <v>109</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
         <v>Sample_7_Control</v>
       </c>
       <c r="E8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F8" t="s">
         <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K8" s="4"/>
       <c r="Q8" s="1"/>
@@ -1777,26 +1697,26 @@
         <v>109</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
         <v>Sample_8_Control</v>
       </c>
       <c r="E9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F9" t="s">
         <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K9" s="4"/>
       <c r="Q9" s="1"/>
@@ -1810,26 +1730,26 @@
         <v>109</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-3 4hr</v>
       </c>
       <c r="E10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F10" t="s">
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K10" s="4"/>
       <c r="Q10" s="1"/>
@@ -1843,26 +1763,26 @@
         <v>109</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
         <v>Sample_10_Control</v>
       </c>
       <c r="E11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
       </c>
       <c r="G11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K11" s="4"/>
       <c r="Q11" s="1"/>
@@ -1876,26 +1796,26 @@
         <v>109</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
         <v>Sample_11_HKDC1</v>
       </c>
       <c r="E12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F12" t="s">
         <v>9</v>
       </c>
       <c r="G12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K12" s="4"/>
       <c r="Q12" s="1"/>
@@ -1909,26 +1829,26 @@
         <v>109</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
         <v>Sample_12_HKDC1</v>
       </c>
       <c r="E13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F13" t="s">
         <v>9</v>
       </c>
       <c r="G13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K13" s="4"/>
       <c r="Q13" s="1"/>
@@ -1942,26 +1862,26 @@
         <v>109</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
         <v>Sample_13_HKDC1</v>
       </c>
       <c r="E14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F14" t="s">
         <v>9</v>
       </c>
       <c r="G14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K14" s="4"/>
       <c r="Q14" s="1"/>
@@ -1975,26 +1895,26 @@
         <v>109</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
         <v>Sample_14_HKDC1</v>
       </c>
       <c r="E15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F15" t="s">
         <v>9</v>
       </c>
       <c r="G15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K15" s="4"/>
       <c r="Q15" s="1"/>
@@ -2008,26 +1928,26 @@
         <v>109</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
         <v>Sample_15_HKDC1</v>
       </c>
       <c r="E16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F16" t="s">
         <v>9</v>
       </c>
       <c r="G16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K16" s="4"/>
       <c r="Q16" s="1"/>
@@ -2041,26 +1961,26 @@
         <v>109</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
         <v>Sample_16_HK1</v>
       </c>
       <c r="E17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F17" t="s">
         <v>9</v>
       </c>
       <c r="G17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K17" s="4"/>
       <c r="Q17" s="1"/>
@@ -2074,26 +1994,26 @@
         <v>109</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
         <v>Sample_17_HK1</v>
       </c>
       <c r="E18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F18" t="s">
         <v>9</v>
       </c>
       <c r="G18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K18" s="4"/>
       <c r="Q18" s="1"/>
@@ -2107,26 +2027,26 @@
         <v>109</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
         <v>Sample_18_HK1</v>
       </c>
       <c r="E19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F19" t="s">
         <v>9</v>
       </c>
       <c r="G19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K19" s="4"/>
       <c r="Q19" s="1"/>
@@ -2140,26 +2060,26 @@
         <v>109</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
         <v>Sample_19_HK1</v>
       </c>
       <c r="E20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F20" t="s">
         <v>9</v>
       </c>
       <c r="G20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K20" s="4"/>
       <c r="Q20" s="1"/>
@@ -2173,26 +2093,26 @@
         <v>109</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
         <v>Sample_20_HK1</v>
       </c>
       <c r="E21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F21" t="s">
         <v>9</v>
       </c>
       <c r="G21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K21" s="4"/>
       <c r="Q21" s="1"/>
@@ -2206,26 +2126,26 @@
         <v>109</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
         <v>Sample_21_GFP</v>
       </c>
       <c r="E22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F22" t="s">
         <v>9</v>
       </c>
       <c r="G22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K22" s="4"/>
       <c r="Q22" s="1"/>
@@ -2239,26 +2159,26 @@
         <v>109</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
         <v>Sample_22_GFP</v>
       </c>
       <c r="E23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F23" t="s">
         <v>9</v>
       </c>
       <c r="G23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K23" s="4"/>
       <c r="Q23" s="1"/>
@@ -2272,26 +2192,26 @@
         <v>109</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
         <v>Sample_23_GFP</v>
       </c>
       <c r="E24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F24" t="s">
         <v>9</v>
       </c>
       <c r="G24" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K24" s="4"/>
       <c r="Q24" s="1"/>
@@ -2305,26 +2225,26 @@
         <v>109</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
         <v>Sample_24_GFP</v>
       </c>
       <c r="E25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F25" t="s">
         <v>9</v>
       </c>
       <c r="G25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K25" s="4"/>
       <c r="Q25" s="1"/>
@@ -2338,26 +2258,26 @@
         <v>109</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
         <v>Sample_25_GFP</v>
       </c>
       <c r="E26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F26" t="s">
         <v>9</v>
       </c>
       <c r="G26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K26" s="4"/>
       <c r="Q26" s="1"/>
@@ -2371,26 +2291,26 @@
         <v>109</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
         <v>Sample_26_Experimental – Fasted State</v>
       </c>
       <c r="E27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F27" t="s">
         <v>9</v>
       </c>
       <c r="G27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K27" s="4"/>
       <c r="Q27" s="1"/>
@@ -2404,26 +2324,26 @@
         <v>109</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
         <v>Sample_27_Experimental – Fasted State</v>
       </c>
       <c r="E28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F28" t="s">
         <v>9</v>
       </c>
       <c r="G28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K28" s="4"/>
       <c r="Q28" s="1"/>
@@ -2437,26 +2357,26 @@
         <v>109</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
         <v>Sample_28_Experimental – Fasted State</v>
       </c>
       <c r="E29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F29" t="s">
         <v>9</v>
       </c>
       <c r="G29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K29" s="4"/>
       <c r="Q29" s="1"/>
@@ -2470,26 +2390,26 @@
         <v>109</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
         <v>Sample_29_Control- Fasted State</v>
       </c>
       <c r="E30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F30" t="s">
         <v>9</v>
       </c>
       <c r="G30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K30" s="4"/>
       <c r="Q30" s="1"/>
@@ -2503,26 +2423,26 @@
         <v>109</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
         <v>Sample_30_Control- Fasted State</v>
       </c>
       <c r="E31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F31" t="s">
         <v>9</v>
       </c>
       <c r="G31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K31" s="4"/>
       <c r="Q31" s="1"/>
@@ -2536,26 +2456,26 @@
         <v>109</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
         <v>Sample_31_Control- Fasted State</v>
       </c>
       <c r="E32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F32" t="s">
         <v>9</v>
       </c>
       <c r="G32" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K32" s="4"/>
       <c r="Q32" s="1"/>
@@ -2569,26 +2489,26 @@
         <v>109</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
         <v>Sample_32_Experimental – Re-fed State</v>
       </c>
       <c r="E33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F33" t="s">
         <v>9</v>
       </c>
       <c r="G33" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K33" s="4"/>
       <c r="Q33" s="1"/>
@@ -2602,26 +2522,26 @@
         <v>109</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
         <v>Sample_33_Experimental – Re-fed State</v>
       </c>
       <c r="E34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F34" t="s">
         <v>9</v>
       </c>
       <c r="G34" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K34" s="4"/>
       <c r="Q34" s="1"/>
@@ -2635,26 +2555,26 @@
         <v>109</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
         <v>Sample_34_Experimental – Re-fed State</v>
       </c>
       <c r="E35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F35" t="s">
         <v>9</v>
       </c>
       <c r="G35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K35" s="4"/>
       <c r="Q35" s="1"/>
@@ -2668,26 +2588,26 @@
         <v>109</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
         <v>Sample_35_Control- Re-fed State</v>
       </c>
       <c r="E36" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F36" t="s">
         <v>9</v>
       </c>
       <c r="G36" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K36" s="4"/>
       <c r="Q36" s="1"/>
@@ -2701,26 +2621,26 @@
         <v>109</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
         <v>Sample_36_Control- Re-fed State</v>
       </c>
       <c r="E37" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F37" t="s">
         <v>9</v>
       </c>
       <c r="G37" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K37" s="4"/>
       <c r="Q37" s="1"/>
@@ -2734,26 +2654,26 @@
         <v>109</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-3 8hr</v>
       </c>
       <c r="E38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F38" t="s">
         <v>9</v>
       </c>
       <c r="G38" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K38" s="4"/>
       <c r="Q38" s="1"/>
@@ -2767,26 +2687,26 @@
         <v>109</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
         <v>Sample_38_Experimental – Fasted State</v>
       </c>
       <c r="E39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F39" t="s">
         <v>9</v>
       </c>
       <c r="G39" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K39" s="4"/>
       <c r="Q39" s="1"/>
@@ -2800,26 +2720,26 @@
         <v>109</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
         <v>Sample_39_Experimental – Fasted State</v>
       </c>
       <c r="E40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F40" t="s">
         <v>9</v>
       </c>
       <c r="G40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K40" s="4"/>
       <c r="Q40" s="1"/>
@@ -2833,26 +2753,26 @@
         <v>109</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="0"/>
         <v>Sample_40_Experimental – Fasted State</v>
       </c>
       <c r="E41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F41" t="s">
         <v>9</v>
       </c>
       <c r="G41" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K41" s="4"/>
       <c r="Q41" s="1"/>
@@ -2866,26 +2786,26 @@
         <v>109</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D42" t="str">
         <f t="shared" si="0"/>
         <v>Sample_41_Control- Fasted State</v>
       </c>
       <c r="E42" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F42" t="s">
         <v>9</v>
       </c>
       <c r="G42" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K42" s="4"/>
       <c r="Q42" s="1"/>
@@ -2899,26 +2819,26 @@
         <v>109</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
         <v>Sample_42_Control- Fasted State</v>
       </c>
       <c r="E43" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F43" t="s">
         <v>9</v>
       </c>
       <c r="G43" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K43" s="4"/>
       <c r="Q43" s="1"/>
@@ -2932,26 +2852,26 @@
         <v>109</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D44" t="str">
         <f t="shared" si="0"/>
         <v>Sample_43_Control- Fasted State</v>
       </c>
       <c r="E44" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F44" t="s">
         <v>9</v>
       </c>
       <c r="G44" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K44" s="4"/>
       <c r="Q44" s="1"/>
@@ -2965,26 +2885,26 @@
         <v>109</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D45" t="str">
         <f t="shared" si="0"/>
         <v>Sample_44_Experimental – Re-fed State</v>
       </c>
       <c r="E45" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F45" t="s">
         <v>9</v>
       </c>
       <c r="G45" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K45" s="4"/>
       <c r="Q45" s="1"/>
@@ -2998,26 +2918,26 @@
         <v>109</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D46" t="str">
         <f t="shared" si="0"/>
         <v>Sample_45_Experimental – Re-fed State</v>
       </c>
       <c r="E46" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F46" t="s">
         <v>9</v>
       </c>
       <c r="G46" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K46" s="4"/>
       <c r="Q46" s="1"/>
@@ -3031,26 +2951,26 @@
         <v>109</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="0"/>
         <v>Sample_46_Experimental – Re-fed State</v>
       </c>
       <c r="E47" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F47" t="s">
         <v>9</v>
       </c>
       <c r="G47" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K47" s="4"/>
       <c r="Q47" s="1"/>
@@ -3064,26 +2984,26 @@
         <v>109</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D48" t="str">
         <f t="shared" si="0"/>
         <v>Sample_47_Control- Re-fed State</v>
       </c>
       <c r="E48" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F48" t="s">
         <v>9</v>
       </c>
       <c r="G48" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K48" s="4"/>
       <c r="Q48" s="1"/>
@@ -3097,26 +3017,26 @@
         <v>109</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D49" t="str">
         <f t="shared" si="0"/>
         <v>Sample_48_Control- Re-fed State</v>
       </c>
       <c r="E49" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F49" t="s">
         <v>9</v>
       </c>
       <c r="G49" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K49" s="4"/>
       <c r="Q49" s="1"/>
@@ -3130,26 +3050,26 @@
         <v>109</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D50" t="str">
         <f t="shared" si="0"/>
         <v>Sample_49_Control- Re-fed State</v>
       </c>
       <c r="E50" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F50" t="s">
         <v>9</v>
       </c>
       <c r="G50" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K50" s="4"/>
       <c r="Q50" s="1"/>
@@ -3163,26 +3083,26 @@
         <v>109</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D51" t="str">
         <f t="shared" si="0"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-1 12hr</v>
       </c>
       <c r="E51" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F51" t="s">
         <v>9</v>
       </c>
       <c r="G51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K51" s="4"/>
       <c r="Q51" s="1"/>
@@ -3196,26 +3116,26 @@
         <v>109</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D52" t="str">
         <f t="shared" si="0"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-1 8hr</v>
       </c>
       <c r="E52" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F52" t="s">
         <v>9</v>
       </c>
       <c r="G52" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K52" s="4"/>
       <c r="Q52" s="1"/>
@@ -3229,26 +3149,26 @@
         <v>109</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D53" t="str">
         <f t="shared" si="0"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-1 4hr</v>
       </c>
       <c r="E53" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F53" t="s">
         <v>9</v>
       </c>
       <c r="G53" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K53" s="4"/>
     </row>
@@ -3260,26 +3180,26 @@
         <v>109</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D54" t="str">
         <f t="shared" si="0"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-1 1hr</v>
       </c>
       <c r="E54" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F54" t="s">
         <v>9</v>
       </c>
       <c r="G54" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K54" s="4"/>
     </row>
@@ -3291,26 +3211,26 @@
         <v>109</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D55" t="str">
         <f t="shared" si="0"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-1 0hr</v>
       </c>
       <c r="E55" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F55" t="s">
         <v>9</v>
       </c>
       <c r="G55" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K55" s="4"/>
     </row>
@@ -3322,26 +3242,26 @@
         <v>109</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D56" t="str">
         <f t="shared" si="0"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-2 12hr</v>
       </c>
       <c r="E56" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F56" t="s">
         <v>9</v>
       </c>
       <c r="G56" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K56" s="4"/>
     </row>
@@ -3353,26 +3273,26 @@
         <v>109</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D57" t="str">
         <f t="shared" si="0"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-2 8hr</v>
       </c>
       <c r="E57" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F57" t="s">
         <v>9</v>
       </c>
       <c r="G57" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K57" s="4"/>
     </row>
@@ -3384,26 +3304,26 @@
         <v>109</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D58" t="str">
         <f t="shared" si="0"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-2 4hr</v>
       </c>
       <c r="E58" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F58" t="s">
         <v>9</v>
       </c>
       <c r="G58" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K58" s="4"/>
     </row>
@@ -3415,26 +3335,26 @@
         <v>109</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D59" t="str">
         <f t="shared" si="0"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-2 1hr</v>
       </c>
       <c r="E59" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F59" t="s">
         <v>9</v>
       </c>
       <c r="G59" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K59" s="4"/>
     </row>
@@ -3446,26 +3366,26 @@
         <v>109</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D60" t="str">
         <f t="shared" si="0"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-2 0hr</v>
       </c>
       <c r="E60" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F60" t="s">
         <v>9</v>
       </c>
       <c r="G60" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K60" s="4"/>
     </row>
@@ -3477,26 +3397,26 @@
         <v>109</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-3 12hr</v>
       </c>
       <c r="E61" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F61" t="s">
         <v>9</v>
       </c>
       <c r="G61" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K61" s="4"/>
     </row>
@@ -3508,29 +3428,29 @@
         <v>109</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
         <v>Sample_H3K4me3_midi_zymo</v>
       </c>
       <c r="E62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F62" t="s">
         <v>9</v>
       </c>
       <c r="G62" t="s">
+        <v>192</v>
+      </c>
+      <c r="H62" t="s">
+        <v>202</v>
+      </c>
+      <c r="I62" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="H62" t="s">
-        <v>203</v>
-      </c>
-      <c r="I62" s="4" t="s">
-        <v>194</v>
-      </c>
       <c r="J62" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K62" s="4"/>
     </row>
@@ -3542,32 +3462,32 @@
         <v>109</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
         <v>Sample_CTCF_midi_zymo</v>
       </c>
       <c r="E63" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F63" t="s">
         <v>9</v>
       </c>
       <c r="G63" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H63" t="s">
         <v>107</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K63" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="64" spans="1:18" ht="19" x14ac:dyDescent="0.25">
@@ -3578,32 +3498,32 @@
         <v>109</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
         <v>Sample_FOSL2_midi_zymo</v>
       </c>
       <c r="E64" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F64" t="s">
         <v>9</v>
       </c>
       <c r="G64" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H64" t="s">
         <v>107</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K64" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="65" spans="1:11" ht="19" x14ac:dyDescent="0.25">
@@ -3614,32 +3534,32 @@
         <v>109</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
         <v>Sample_JunB_midi_zymo</v>
       </c>
       <c r="E65" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F65" t="s">
         <v>9</v>
       </c>
       <c r="G65" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H65" t="s">
         <v>107</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K65" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="66" spans="1:11" ht="19" x14ac:dyDescent="0.25">
@@ -3650,29 +3570,29 @@
         <v>109</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D66" t="str">
         <f t="shared" si="0"/>
         <v>Sample_H3K4me3_deep_zymo</v>
       </c>
       <c r="E66" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F66" t="s">
         <v>9</v>
       </c>
       <c r="G66" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H66" t="s">
         <v>107</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K66" s="4"/>
     </row>
@@ -3684,29 +3604,29 @@
         <v>109</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D67" t="str">
         <f t="shared" si="0"/>
         <v>Sample_CTCF_deep_zymo</v>
       </c>
       <c r="E67" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F67" t="s">
         <v>9</v>
       </c>
       <c r="G67" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H67" t="s">
         <v>107</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K67" s="4"/>
     </row>
@@ -3718,29 +3638,29 @@
         <v>109</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D68" t="str">
         <f t="shared" ref="D68:D95" si="1">CONCATENATE("Sample_",E68,"")</f>
         <v>Sample_FOSL2_deep_zymo</v>
       </c>
       <c r="E68" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F68" t="s">
         <v>9</v>
       </c>
       <c r="G68" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H68" t="s">
         <v>107</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K68" s="4"/>
     </row>
@@ -3752,29 +3672,29 @@
         <v>109</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D69" t="str">
         <f t="shared" si="1"/>
         <v>Sample_JunB_deep_zymo</v>
       </c>
       <c r="E69" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F69" t="s">
         <v>9</v>
       </c>
       <c r="G69" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H69" t="s">
         <v>107</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K69" s="4"/>
     </row>
@@ -3786,29 +3706,29 @@
         <v>109</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D70" t="str">
         <f t="shared" si="1"/>
         <v>Sample_H3K4me3_midi_qiagen</v>
       </c>
       <c r="E70" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F70" t="s">
         <v>9</v>
       </c>
       <c r="G70" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H70" t="s">
         <v>107</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K70" s="4"/>
     </row>
@@ -3820,29 +3740,29 @@
         <v>109</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D71" t="str">
         <f t="shared" si="1"/>
         <v>Sample_CTCF_midi_qiagen</v>
       </c>
       <c r="E71" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F71" t="s">
         <v>9</v>
       </c>
       <c r="G71" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H71" t="s">
         <v>107</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K71" s="4"/>
     </row>
@@ -3854,29 +3774,29 @@
         <v>109</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D72" t="str">
         <f t="shared" si="1"/>
         <v>Sample_FOSL2_midi_qiagen</v>
       </c>
       <c r="E72" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F72" t="s">
         <v>9</v>
       </c>
       <c r="G72" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H72" t="s">
         <v>107</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K72" s="4"/>
     </row>
@@ -3888,29 +3808,29 @@
         <v>109</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="1"/>
         <v>Sample_JunB_midi_qiagen</v>
       </c>
       <c r="E73" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F73" t="s">
         <v>9</v>
       </c>
       <c r="G73" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H73" t="s">
         <v>107</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K73" s="4"/>
     </row>
@@ -3922,29 +3842,29 @@
         <v>109</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D74" t="str">
         <f t="shared" si="1"/>
         <v>Sample_H3K4me3_deep_qiagen</v>
       </c>
       <c r="E74" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F74" t="s">
         <v>9</v>
       </c>
       <c r="G74" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H74" t="s">
         <v>107</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K74" s="4"/>
     </row>
@@ -3956,29 +3876,29 @@
         <v>109</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D75" t="str">
         <f t="shared" si="1"/>
         <v>Sample_CTCF_deep_qiagen</v>
       </c>
       <c r="E75" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F75" t="s">
         <v>9</v>
       </c>
       <c r="G75" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H75" t="s">
         <v>107</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K75" s="4"/>
     </row>
@@ -3990,29 +3910,29 @@
         <v>109</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D76" t="str">
         <f t="shared" si="1"/>
         <v>Sample_FOSL2_deep_qiagen</v>
       </c>
       <c r="E76" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F76" t="s">
         <v>9</v>
       </c>
       <c r="G76" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H76" t="s">
         <v>107</v>
       </c>
       <c r="I76" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K76" s="4"/>
     </row>
@@ -4024,29 +3944,29 @@
         <v>109</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D77" t="str">
         <f t="shared" si="1"/>
         <v>Sample_JunB_deep_qiagen</v>
       </c>
       <c r="E77" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F77" t="s">
         <v>9</v>
       </c>
       <c r="G77" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H77" t="s">
         <v>107</v>
       </c>
       <c r="I77" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J77" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K77" s="4"/>
     </row>
@@ -4058,29 +3978,29 @@
         <v>109</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D78" t="str">
         <f t="shared" si="1"/>
         <v>Sample_SL_GR_sc12763x</v>
       </c>
       <c r="E78" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F78" t="s">
         <v>9</v>
       </c>
       <c r="G78" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H78" t="s">
         <v>107</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J78" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K78" s="4"/>
     </row>
@@ -4092,29 +4012,29 @@
         <v>109</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D79" t="str">
         <f t="shared" si="1"/>
         <v>Sample_SL_GR_136209</v>
       </c>
       <c r="E79" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F79" t="s">
         <v>9</v>
       </c>
       <c r="G79" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H79" t="s">
         <v>107</v>
       </c>
       <c r="I79" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J79" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K79" s="4"/>
     </row>
@@ -4126,29 +4046,29 @@
         <v>109</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D80" t="str">
         <f t="shared" si="1"/>
         <v>Sample_SL_GR_MA1510</v>
       </c>
       <c r="E80" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F80" t="s">
         <v>9</v>
       </c>
       <c r="G80" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H80" t="s">
         <v>107</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K80" s="4"/>
     </row>
@@ -4160,29 +4080,29 @@
         <v>109</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D81" t="str">
         <f t="shared" si="1"/>
         <v>Sample_SL_Ipctrl_H3K27ac</v>
       </c>
       <c r="E81" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F81" t="s">
         <v>9</v>
       </c>
       <c r="G81" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H81" t="s">
         <v>107</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K81" s="4"/>
     </row>
@@ -4194,29 +4114,29 @@
         <v>109</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="1"/>
         <v>Sample_mouse_liver_TD_method_Input_Ctrl</v>
       </c>
       <c r="E82" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F82" t="s">
         <v>9</v>
       </c>
       <c r="G82" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H82" t="s">
         <v>107</v>
       </c>
       <c r="I82" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K82" s="4"/>
     </row>
@@ -4228,29 +4148,29 @@
         <v>109</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D83" t="str">
         <f t="shared" si="1"/>
         <v>Sample_mouse_liver_LH_method_Input_Ctrl</v>
       </c>
       <c r="E83" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F83" t="s">
         <v>9</v>
       </c>
       <c r="G83" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H83" t="s">
         <v>107</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K83" s="4"/>
     </row>
@@ -4262,26 +4182,26 @@
         <v>109</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D84" t="str">
         <f t="shared" si="1"/>
         <v>Sample_49_Control- Re-fed State</v>
       </c>
       <c r="E84" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F84" t="s">
         <v>9</v>
       </c>
       <c r="G84" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I84" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K84" s="4"/>
     </row>
@@ -4293,26 +4213,26 @@
         <v>109</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D85" t="str">
         <f t="shared" si="1"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-1 12hr</v>
       </c>
       <c r="E85" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F85" t="s">
         <v>9</v>
       </c>
       <c r="G85" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I85" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K85" s="4"/>
     </row>
@@ -4324,26 +4244,26 @@
         <v>109</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D86" t="str">
         <f t="shared" si="1"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-1 8hr</v>
       </c>
       <c r="E86" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F86" t="s">
         <v>9</v>
       </c>
       <c r="G86" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I86" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J86" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K86" s="4"/>
     </row>
@@ -4355,26 +4275,26 @@
         <v>109</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D87" t="str">
         <f t="shared" si="1"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-1 4hr</v>
       </c>
       <c r="E87" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F87" t="s">
         <v>9</v>
       </c>
       <c r="G87" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K87" s="4"/>
     </row>
@@ -4386,26 +4306,26 @@
         <v>109</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D88" t="str">
         <f t="shared" si="1"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-1 1hr</v>
       </c>
       <c r="E88" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F88" t="s">
         <v>9</v>
       </c>
       <c r="G88" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J88" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K88" s="4"/>
     </row>
@@ -4417,26 +4337,26 @@
         <v>109</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D89" t="str">
         <f t="shared" si="1"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-1 0hr</v>
       </c>
       <c r="E89" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F89" t="s">
         <v>9</v>
       </c>
       <c r="G89" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J89" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K89" s="4"/>
       <c r="L89" s="3"/>
@@ -4449,26 +4369,26 @@
         <v>109</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D90" t="str">
         <f t="shared" si="1"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-2 12hr</v>
       </c>
       <c r="E90" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F90" t="s">
         <v>9</v>
       </c>
       <c r="G90" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I90" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J90" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K90" s="4"/>
       <c r="L90" s="3"/>
@@ -4481,26 +4401,26 @@
         <v>109</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D91" t="str">
         <f t="shared" si="1"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-2 8hr</v>
       </c>
       <c r="E91" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F91" t="s">
         <v>9</v>
       </c>
       <c r="G91" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I91" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J91" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K91" s="4"/>
       <c r="L91" s="3"/>
@@ -4513,26 +4433,26 @@
         <v>109</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D92" t="str">
         <f t="shared" si="1"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-2 4hr</v>
       </c>
       <c r="E92" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F92" t="s">
         <v>9</v>
       </c>
       <c r="G92" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I92" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J92" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K92" s="4"/>
       <c r="L92" s="3"/>
@@ -4545,26 +4465,26 @@
         <v>109</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D93" t="str">
         <f t="shared" si="1"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-2 1hr</v>
       </c>
       <c r="E93" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F93" t="s">
         <v>9</v>
       </c>
       <c r="G93" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I93" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K93" s="4"/>
       <c r="L93" s="3"/>
@@ -4577,26 +4497,26 @@
         <v>109</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D94" t="str">
         <f t="shared" si="1"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-2 0hr</v>
       </c>
       <c r="E94" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F94" t="s">
         <v>9</v>
       </c>
       <c r="G94" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I94" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J94" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K94" s="4"/>
       <c r="L94" s="3"/>
@@ -4609,26 +4529,26 @@
         <v>109</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>110</v>
+        <v>203</v>
       </c>
       <c r="D95" t="str">
         <f t="shared" si="1"/>
         <v>Sample_GR-FLAG 2/27/17 biorep 1-3 12hr</v>
       </c>
       <c r="E95" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F95" t="s">
         <v>9</v>
       </c>
       <c r="G95" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I95" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K95" s="4"/>
       <c r="L95" s="3"/>
@@ -4647,26 +4567,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="160406">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="160406">
       <formula>NOT(ISERROR(SEARCH("160406",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="160604">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="160604">
       <formula>NOT(ISERROR(SEARCH("160604",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K4">
-    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="160406">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="160406">
       <formula>NOT(ISERROR(SEARCH("160406",K2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="160604">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="160604">
       <formula>NOT(ISERROR(SEARCH("160604",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K63:K65">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="160406">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="160406">
       <formula>NOT(ISERROR(SEARCH("160406",K63)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="160604">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="160604">
       <formula>NOT(ISERROR(SEARCH("160604",K63)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>